<commit_message>
Update single network scenario result to use excel
</commit_message>
<xml_diff>
--- a/examples/palabra/results.xlsx
+++ b/examples/palabra/results.xlsx
@@ -817,10 +817,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C4" t="n">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D4" t="n">
         <v>399</v>
@@ -848,55 +848,55 @@
 19: `3.2.0.2` not reachable from device `as1r1`.
 20: `1.0.0.2` not reachable from device `as1r2`.
 21: `2.1.0.2` not reachable from device `as1r2`.
-22: `3.1.0.2` not reachable from device `as1r2`.
-23: `3.2.0.1` not reachable from device `as1r2`.
-24: `3.2.0.2` not reachable from device `as1r2`.
-25: `1.0.0.2` not reachable from device `as2r1`.
-26: `2.1.0.2` not reachable from device `as2r1`.
-27: `3.1.0.2` not reachable from device `as2r1`.
-28: `3.2.0.1` not reachable from device `as2r1`.
-29: `3.2.0.2` not reachable from device `as2r1`.
-30: `1.0.0.2` not reachable from device `as2r2`.
-31: `2.1.0.2` not reachable from device `as2r2`.
-32: `3.1.0.2` not reachable from device `as2r2`.
-33: `3.2.0.1` not reachable from device `as2r2`.
-34: `3.2.0.2` not reachable from device `as2r2`.
-35: `1.0.0.2` not reachable from device `as3r1`.
-36: `2.1.0.2` not reachable from device `as3r1`.
-37: `3.1.0.2` not reachable from device `as3r1`.
-38: `3.2.0.1` not reachable from device `as3r1`.
-39: `3.2.0.2` not reachable from device `as3r1`.
-40: `1.0.0.2` not reachable from device `as3r2`.
-41: `2.1.0.2` not reachable from device `as3r2`.
-42: `3.1.0.2` not reachable from device `as3r2`.
-43: `3.2.0.1` not reachable from device `as3r2`.
-44: `3.2.0.2` not reachable from device `as3r2`.
-45: `1.0.0.1` not reachable from device `local`.
-46: `1.0.0.2` not reachable from device `local`.
-47: `1.1.0.1` not reachable from device `local`.
-48: `1.1.0.2` not reachable from device `local`.
-49: `2.0.0.1` not reachable from device `local`.
-50: `2.0.0.2` not reachable from device `local`.
-51: `2.1.0.1` not reachable from device `local`.
-52: `2.1.0.2` not reachable from device `local`.
-53: `3.0.0.1` not reachable from device `local`.
-54: `3.0.0.2` not reachable from device `local`.
-55: `3.1.0.1` not reachable from device `local`.
-56: `3.1.0.2` not reachable from device `local`.
-57: `3.2.0.1` not reachable from device `local`.
-58: `3.2.0.2` not reachable from device `local`.
-59: `10.20.0.1` not reachable from device `local`.
-60: `10.20.0.2` not reachable from device `local`.
-61: `10.20.1.1` not reachable from device `local`.
-62: `10.20.1.2` not reachable from device `local`.
-63: `20.30.0.1` not reachable from device `local`.
-64: `20.30.0.2` not reachable from device `local`.
-65: `20.30.1.1` not reachable from device `local`.
-66: `20.30.1.2` not reachable from device `local`.
-67: Device `root` is not running.
-68: Device `root` is not running.
-69: Device `root` is not running.
-70: Device `root` is not running.
+22: `3.1.0.1` not reachable from device `as1r2`.
+23: `3.1.0.2` not reachable from device `as1r2`.
+24: `3.2.0.1` not reachable from device `as1r2`.
+25: `3.2.0.2` not reachable from device `as1r2`.
+26: `20.30.0.1` not reachable from device `as1r2`.
+27: `1.0.0.2` not reachable from device `as2r1`.
+28: `2.1.0.2` not reachable from device `as2r1`.
+29: `3.1.0.2` not reachable from device `as2r1`.
+30: `3.2.0.1` not reachable from device `as2r1`.
+31: `3.2.0.2` not reachable from device `as2r1`.
+32: `20.30.1.1` not reachable from device `as2r1`.
+33: `1.0.0.2` not reachable from device `as2r2`.
+34: `2.1.0.2` not reachable from device `as2r2`.
+35: `3.1.0.1` not reachable from device `as2r2`.
+36: `3.1.0.2` not reachable from device `as2r2`.
+37: `3.2.0.1` not reachable from device `as2r2`.
+38: `3.2.0.2` not reachable from device `as2r2`.
+39: `1.0.0.2` not reachable from device `as3r1`.
+40: `2.1.0.2` not reachable from device `as3r1`.
+41: `3.1.0.2` not reachable from device `as3r1`.
+42: `3.2.0.1` not reachable from device `as3r1`.
+43: `3.2.0.2` not reachable from device `as3r1`.
+44: `1.0.0.2` not reachable from device `as3r2`.
+45: `2.1.0.2` not reachable from device `as3r2`.
+46: `3.1.0.2` not reachable from device `as3r2`.
+47: `3.2.0.1` not reachable from device `as3r2`.
+48: `3.2.0.2` not reachable from device `as3r2`.
+49: `1.0.0.1` not reachable from device `local`.
+50: `1.0.0.2` not reachable from device `local`.
+51: `1.1.0.1` not reachable from device `local`.
+52: `1.1.0.2` not reachable from device `local`.
+53: `2.0.0.1` not reachable from device `local`.
+54: `2.0.0.2` not reachable from device `local`.
+55: `2.1.0.1` not reachable from device `local`.
+56: `2.1.0.2` not reachable from device `local`.
+57: `3.0.0.1` not reachable from device `local`.
+58: `3.0.0.2` not reachable from device `local`.
+59: `3.1.0.1` not reachable from device `local`.
+60: `3.1.0.2` not reachable from device `local`.
+61: `3.2.0.1` not reachable from device `local`.
+62: `3.2.0.2` not reachable from device `local`.
+63: `10.20.0.1` not reachable from device `local`.
+64: `10.20.0.2` not reachable from device `local`.
+65: `10.20.1.1` not reachable from device `local`.
+66: `10.20.1.2` not reachable from device `local`.
+67: `20.30.0.1` not reachable from device `local`.
+68: `20.30.0.2` not reachable from device `local`.
+69: `20.30.1.1` not reachable from device `local`.
+70: `20.30.1.2` not reachable from device `local`.
 71: Device `root` is not running.
 72: Device `root` is not running.
 73: Device `root` is not running.
@@ -915,10 +915,10 @@
 86: Device `root` is not running.
 87: Device `root` is not running.
 88: Device `root` is not running.
-89: Device `net` is not running.
-90: Device `net` is not running.
-91: Device `net` is not running.
-92: Device `net` is not running.
+89: Device `root` is not running.
+90: Device `root` is not running.
+91: Device `root` is not running.
+92: Device `root` is not running.
 93: Device `net` is not running.
 94: Device `net` is not running.
 95: Device `net` is not running.
@@ -937,58 +937,62 @@
 108: Device `net` is not running.
 109: Device `net` is not running.
 110: Device `net` is not running.
-111: `1.1.0.1` not reachable from device `pc`.
-112: `1.1.0.2` not reachable from device `pc`.
-113: `2.0.0.1` not reachable from device `pc`.
-114: `2.0.0.2` not reachable from device `pc`.
-115: `2.1.0.1` not reachable from device `pc`.
-116: `2.1.0.2` not reachable from device `pc`.
-117: `3.0.0.1` not reachable from device `pc`.
-118: `3.0.0.2` not reachable from device `pc`.
-119: `3.1.0.1` not reachable from device `pc`.
-120: `3.1.0.2` not reachable from device `pc`.
-121: `3.2.0.1` not reachable from device `pc`.
-122: `3.2.0.2` not reachable from device `pc`.
-123: `10.20.0.1` not reachable from device `pc`.
-124: `10.20.0.2` not reachable from device `pc`.
-125: `10.20.1.1` not reachable from device `pc`.
-126: `10.20.1.2` not reachable from device `pc`.
-127: `20.30.0.1` not reachable from device `pc`.
-128: `20.30.0.2` not reachable from device `pc`.
-129: `20.30.1.1` not reachable from device `pc`.
-130: `20.30.1.2` not reachable from device `pc`.
-131: Device net not in the network scenario.
-132: Device net not in the network scenario.
-133: Device root not in the network scenario.
-134: Device root not in the network scenario.
-135: The peering between as1r1 and 1.0.0.2 is not up.
-136: The peering between as1r2 and 1.0.0.1 is not up.
-137: The route 3.2.0.0/24 IS NOT found in the routing table of `as3r1`.
-138: The route 0.0.0.0/0 IS NOT found in the routing table of `root`.
-139: The route 1.1.0.0/24 IS NOT found in the routing table of `root`.
-140: The route 0.0.0.0/0 IS NOT found in the routing table of `net`.
-141: The route 2.1.0.0/24 IS NOT found in the routing table of `net`.
-142: The route 0.0.0.0/0 IS NOT found in the routing table of `pc`.
-143: The route 3.1.0.0/24 IS NOT found in the routing table of `pc`.
-144: The route 0.0.0.0/0 IS NOT found in the routing table of `local`.
-145: The route 3.2.0.0/24 IS NOT found in the routing table of `local`.
-146: Device `root` is not running.
-147: Device `root` is not running.
-148: named on local is running but answered with REFUSED when quering for .
-149: Device `net` is not running.
-150: `resolv.conf` file not found for device `as1r1`
-151: `resolv.conf` file not found for device `as1r2`
-152: `resolv.conf` file not found for device `as2r1`
-153: `resolv.conf` file not found for device `as2r2`
-154: `resolv.conf` file not found for device `as3r1`
-155: `resolv.conf` file not found for device `as3r2`
-156: The local name server for device `pc` has ip `3.2.0.2`
-157: `pc.net` not reachable from device `as1r1`.
-158: `pc.net` not reachable from device `as1r2`.
-159: `pc.net` not reachable from device `as2r1`.
-160: `pc.net` not reachable from device `as2r2`.
-161: `pc.net` not reachable from device `as3r1`.
-162: `pc.net` not reachable from device `as3r2`.
+111: Device `net` is not running.
+112: Device `net` is not running.
+113: Device `net` is not running.
+114: Device `net` is not running.
+115: `1.1.0.1` not reachable from device `pc`.
+116: `1.1.0.2` not reachable from device `pc`.
+117: `2.0.0.1` not reachable from device `pc`.
+118: `2.0.0.2` not reachable from device `pc`.
+119: `2.1.0.1` not reachable from device `pc`.
+120: `2.1.0.2` not reachable from device `pc`.
+121: `3.0.0.1` not reachable from device `pc`.
+122: `3.0.0.2` not reachable from device `pc`.
+123: `3.1.0.1` not reachable from device `pc`.
+124: `3.1.0.2` not reachable from device `pc`.
+125: `3.2.0.1` not reachable from device `pc`.
+126: `3.2.0.2` not reachable from device `pc`.
+127: `10.20.0.1` not reachable from device `pc`.
+128: `10.20.0.2` not reachable from device `pc`.
+129: `10.20.1.1` not reachable from device `pc`.
+130: `10.20.1.2` not reachable from device `pc`.
+131: `20.30.0.1` not reachable from device `pc`.
+132: `20.30.0.2` not reachable from device `pc`.
+133: `20.30.1.1` not reachable from device `pc`.
+134: `20.30.1.2` not reachable from device `pc`.
+135: Device net not in the network scenario.
+136: Device net not in the network scenario.
+137: Device root not in the network scenario.
+138: Device root not in the network scenario.
+139: The peering between as1r1 and 1.0.0.2 is not up.
+140: The peering between as1r2 and 1.0.0.1 is not up.
+141: The route 3.2.0.0/24 IS NOT found in the routing table of `as3r1`.
+142: The route 0.0.0.0/0 IS NOT found in the routing table of `root`.
+143: The route 1.1.0.0/24 IS NOT found in the routing table of `root`.
+144: The route 0.0.0.0/0 IS NOT found in the routing table of `net`.
+145: The route 2.1.0.0/24 IS NOT found in the routing table of `net`.
+146: The route 0.0.0.0/0 IS NOT found in the routing table of `pc`.
+147: The route 3.1.0.0/24 IS NOT found in the routing table of `pc`.
+148: The route 0.0.0.0/0 IS NOT found in the routing table of `local`.
+149: The route 3.2.0.0/24 IS NOT found in the routing table of `local`.
+150: Device `root` is not running.
+151: Device `root` is not running.
+152: named on local is running but answered with REFUSED when quering for .
+153: Device `net` is not running.
+154: `resolv.conf` file not found for device `as1r1`
+155: `resolv.conf` file not found for device `as1r2`
+156: `resolv.conf` file not found for device `as2r1`
+157: `resolv.conf` file not found for device `as2r2`
+158: `resolv.conf` file not found for device `as3r1`
+159: `resolv.conf` file not found for device `as3r2`
+160: The local name server for device `pc` has ip `3.2.0.2`
+161: `pc.net` not reachable from device `as1r1`.
+162: `pc.net` not reachable from device `as1r2`.
+163: `pc.net` not reachable from device `as2r1`.
+164: `pc.net` not reachable from device `as2r2`.
+165: `pc.net` not reachable from device `as3r1`.
+166: `pc.net` not reachable from device `as3r2`.
 </t>
         </is>
       </c>

</xml_diff>